<commit_message>
New Tests for Smoke
</commit_message>
<xml_diff>
--- a/cypress/downloads/ClinicActivity-04_04_2024.xlsx
+++ b/cypress/downloads/ClinicActivity-04_04_2024.xlsx
@@ -5,10 +5,10 @@
     <workbookView tabRatio="600"/>
   </bookViews>
   <sheets>
-    <sheet name="Automation Tests" sheetId="1" r:id="R9823cc51e17e4af0"/>
-    <sheet name="Automation Engineer" sheetId="2" r:id="Raabb9e3ba0d14a93"/>
-    <sheet name="Automation Another" sheetId="3" r:id="Ra9e9173eb8ba4ba0"/>
-    <sheet name="Help Desk Help Desk" sheetId="4" r:id="R5bd3c19664d64328"/>
+    <sheet name="Automation Tests" sheetId="1" r:id="Ra738e7a5385e46a4"/>
+    <sheet name="Automation Engineer" sheetId="2" r:id="Rae49289fc7014377"/>
+    <sheet name="Automation Another" sheetId="3" r:id="R5a558544f5f84b57"/>
+    <sheet name="Help Desk Help Desk" sheetId="4" r:id="R083959f817d94893"/>
   </sheets>
 </workbook>
 </file>
@@ -3376,7 +3376,7 @@
         <v>Automation Engineer</v>
       </c>
       <c t="str">
-        <v>544</v>
+        <v>551</v>
       </c>
       <c t="str">
         <v>0</v>
@@ -3475,6 +3475,38 @@
         <v>4/8/2024</v>
       </c>
       <c t="str">
+        <v>Test First Name Field Test Last Name Field</v>
+      </c>
+      <c t="str">
+        <v>4/13/2024</v>
+      </c>
+      <c t="str">
+        <v>Appointment</v>
+      </c>
+      <c t="str">
+        <v>Automation with CCPE</v>
+      </c>
+      <c t="str">
+        <v>$0.00</v>
+      </c>
+      <c t="str">
+        <v>$0.00</v>
+      </c>
+      <c t="str">
+        <v>$0.00</v>
+      </c>
+      <c t="str">
+        <v>$0.00</v>
+      </c>
+      <c t="str">
+        <v>$0.00</v>
+      </c>
+    </row>
+    <row>
+      <c t="str">
+        <v>4/8/2024</v>
+      </c>
+      <c t="str">
         <v>Automation  Engineer E</v>
       </c>
       <c t="str">
@@ -3923,6 +3955,102 @@
         <v>4/8/2024</v>
       </c>
       <c t="str">
+        <v>Automation  Engineer E</v>
+      </c>
+      <c t="str">
+        <v>4/3/2024</v>
+      </c>
+      <c t="str">
+        <v>Appointment</v>
+      </c>
+      <c t="str">
+        <v>Automation with CCPE</v>
+      </c>
+      <c t="str">
+        <v>$0.00</v>
+      </c>
+      <c t="str">
+        <v>$0.00</v>
+      </c>
+      <c t="str">
+        <v>$0.00</v>
+      </c>
+      <c t="str">
+        <v>$0.00</v>
+      </c>
+      <c t="str">
+        <v>$0.00</v>
+      </c>
+    </row>
+    <row>
+      <c t="str">
+        <v>4/8/2024</v>
+      </c>
+      <c t="str">
+        <v>Automation  Engineer E</v>
+      </c>
+      <c t="str">
+        <v>4/3/2024</v>
+      </c>
+      <c t="str">
+        <v>Appointment</v>
+      </c>
+      <c t="str">
+        <v>Automation with CCPE</v>
+      </c>
+      <c t="str">
+        <v>$0.00</v>
+      </c>
+      <c t="str">
+        <v>$0.00</v>
+      </c>
+      <c t="str">
+        <v>$0.00</v>
+      </c>
+      <c t="str">
+        <v>$0.00</v>
+      </c>
+      <c t="str">
+        <v>$0.00</v>
+      </c>
+    </row>
+    <row>
+      <c t="str">
+        <v>4/8/2024</v>
+      </c>
+      <c t="str">
+        <v>Automation  Engineer E</v>
+      </c>
+      <c t="str">
+        <v>4/3/2024</v>
+      </c>
+      <c t="str">
+        <v>Appointment</v>
+      </c>
+      <c t="str">
+        <v>Automation with CCPE</v>
+      </c>
+      <c t="str">
+        <v>$0.00</v>
+      </c>
+      <c t="str">
+        <v>$0.00</v>
+      </c>
+      <c t="str">
+        <v>$0.00</v>
+      </c>
+      <c t="str">
+        <v>$0.00</v>
+      </c>
+      <c t="str">
+        <v>$0.00</v>
+      </c>
+    </row>
+    <row>
+      <c t="str">
+        <v>4/8/2024</v>
+      </c>
+      <c t="str">
         <v>Test First Name Field Test Last Name Field</v>
       </c>
       <c t="str">
@@ -6198,6 +6326,38 @@
         <v>Test First Name Field Test Last Name Field</v>
       </c>
       <c t="str">
+        <v>4/13/2024</v>
+      </c>
+      <c t="str">
+        <v>Appointment</v>
+      </c>
+      <c t="str">
+        <v>Automation with CCPE</v>
+      </c>
+      <c t="str">
+        <v>$0.00</v>
+      </c>
+      <c t="str">
+        <v>$0.00</v>
+      </c>
+      <c t="str">
+        <v>$0.00</v>
+      </c>
+      <c t="str">
+        <v>$0.00</v>
+      </c>
+      <c t="str">
+        <v>$0.00</v>
+      </c>
+    </row>
+    <row>
+      <c t="str">
+        <v>4/8/2024</v>
+      </c>
+      <c t="str">
+        <v>Test First Name Field Test Last Name Field</v>
+      </c>
+      <c t="str">
         <v>4/10/2024</v>
       </c>
       <c t="str">
@@ -7379,6 +7539,70 @@
         <v>4/8/2024</v>
       </c>
       <c t="str">
+        <v>Automation  Engineer E</v>
+      </c>
+      <c t="str">
+        <v>4/3/2024</v>
+      </c>
+      <c t="str">
+        <v>Appointment</v>
+      </c>
+      <c t="str">
+        <v>Automation with CCPE</v>
+      </c>
+      <c t="str">
+        <v>$0.00</v>
+      </c>
+      <c t="str">
+        <v>$0.00</v>
+      </c>
+      <c t="str">
+        <v>$0.00</v>
+      </c>
+      <c t="str">
+        <v>$0.00</v>
+      </c>
+      <c t="str">
+        <v>$0.00</v>
+      </c>
+    </row>
+    <row>
+      <c t="str">
+        <v>4/8/2024</v>
+      </c>
+      <c t="str">
+        <v>Automation  Engineer E</v>
+      </c>
+      <c t="str">
+        <v>4/3/2024</v>
+      </c>
+      <c t="str">
+        <v>Appointment</v>
+      </c>
+      <c t="str">
+        <v>Automation with CCPE</v>
+      </c>
+      <c t="str">
+        <v>$0.00</v>
+      </c>
+      <c t="str">
+        <v>$0.00</v>
+      </c>
+      <c t="str">
+        <v>$0.00</v>
+      </c>
+      <c t="str">
+        <v>$0.00</v>
+      </c>
+      <c t="str">
+        <v>$0.00</v>
+      </c>
+    </row>
+    <row>
+      <c t="str">
+        <v>4/8/2024</v>
+      </c>
+      <c t="str">
         <v>Test First Name Field Test Last Name Field</v>
       </c>
       <c t="str">
@@ -20973,6 +21197,93 @@
         <v>4/8/2024</v>
       </c>
       <c t="str">
+        <v>Test First Name Field Test Last Name Field</v>
+      </c>
+      <c t="str">
+        <v>4/13/2024</v>
+      </c>
+      <c t="str">
+        <v>Service</v>
+      </c>
+      <c t="str">
+        <v/>
+      </c>
+      <c t="str">
+        <v/>
+      </c>
+      <c t="str">
+        <v>$0</v>
+      </c>
+      <c t="str">
+        <v>$0</v>
+      </c>
+      <c t="str">
+        <v>$0</v>
+      </c>
+    </row>
+    <row>
+      <c t="str">
+        <v>4/8/2024</v>
+      </c>
+      <c t="str">
+        <v>Test First Name Field Test Last Name Field</v>
+      </c>
+      <c t="str">
+        <v>4/13/2024</v>
+      </c>
+      <c t="str">
+        <v>Product</v>
+      </c>
+      <c t="str">
+        <v/>
+      </c>
+      <c t="str">
+        <v/>
+      </c>
+      <c t="str">
+        <v>$0</v>
+      </c>
+      <c t="str">
+        <v>$0</v>
+      </c>
+      <c t="str">
+        <v>$0</v>
+      </c>
+    </row>
+    <row>
+      <c t="str">
+        <v/>
+      </c>
+      <c t="str">
+        <v/>
+      </c>
+      <c t="str">
+        <v/>
+      </c>
+      <c t="str">
+        <v/>
+      </c>
+      <c t="str">
+        <v/>
+      </c>
+      <c t="str">
+        <v/>
+      </c>
+      <c t="str">
+        <v/>
+      </c>
+      <c t="str">
+        <v/>
+      </c>
+      <c t="str">
+        <v/>
+      </c>
+    </row>
+    <row>
+      <c t="str">
+        <v>4/8/2024</v>
+      </c>
+      <c t="str">
         <v>Automation  Engineer E</v>
       </c>
       <c t="str">
@@ -22191,6 +22502,267 @@
         <v>4/8/2024</v>
       </c>
       <c t="str">
+        <v>Automation  Engineer E</v>
+      </c>
+      <c t="str">
+        <v>4/3/2024</v>
+      </c>
+      <c t="str">
+        <v>Service</v>
+      </c>
+      <c t="str">
+        <v/>
+      </c>
+      <c t="str">
+        <v/>
+      </c>
+      <c t="str">
+        <v>$0</v>
+      </c>
+      <c t="str">
+        <v>$0</v>
+      </c>
+      <c t="str">
+        <v>$0</v>
+      </c>
+    </row>
+    <row>
+      <c t="str">
+        <v>4/8/2024</v>
+      </c>
+      <c t="str">
+        <v>Automation  Engineer E</v>
+      </c>
+      <c t="str">
+        <v>4/3/2024</v>
+      </c>
+      <c t="str">
+        <v>Product</v>
+      </c>
+      <c t="str">
+        <v/>
+      </c>
+      <c t="str">
+        <v/>
+      </c>
+      <c t="str">
+        <v>$0</v>
+      </c>
+      <c t="str">
+        <v>$0</v>
+      </c>
+      <c t="str">
+        <v>$0</v>
+      </c>
+    </row>
+    <row>
+      <c t="str">
+        <v/>
+      </c>
+      <c t="str">
+        <v/>
+      </c>
+      <c t="str">
+        <v/>
+      </c>
+      <c t="str">
+        <v/>
+      </c>
+      <c t="str">
+        <v/>
+      </c>
+      <c t="str">
+        <v/>
+      </c>
+      <c t="str">
+        <v/>
+      </c>
+      <c t="str">
+        <v/>
+      </c>
+      <c t="str">
+        <v/>
+      </c>
+    </row>
+    <row>
+      <c t="str">
+        <v>4/8/2024</v>
+      </c>
+      <c t="str">
+        <v>Automation  Engineer E</v>
+      </c>
+      <c t="str">
+        <v>4/3/2024</v>
+      </c>
+      <c t="str">
+        <v>Service</v>
+      </c>
+      <c t="str">
+        <v/>
+      </c>
+      <c t="str">
+        <v/>
+      </c>
+      <c t="str">
+        <v>$0</v>
+      </c>
+      <c t="str">
+        <v>$0</v>
+      </c>
+      <c t="str">
+        <v>$0</v>
+      </c>
+    </row>
+    <row>
+      <c t="str">
+        <v>4/8/2024</v>
+      </c>
+      <c t="str">
+        <v>Automation  Engineer E</v>
+      </c>
+      <c t="str">
+        <v>4/3/2024</v>
+      </c>
+      <c t="str">
+        <v>Product</v>
+      </c>
+      <c t="str">
+        <v/>
+      </c>
+      <c t="str">
+        <v/>
+      </c>
+      <c t="str">
+        <v>$0</v>
+      </c>
+      <c t="str">
+        <v>$0</v>
+      </c>
+      <c t="str">
+        <v>$0</v>
+      </c>
+    </row>
+    <row>
+      <c t="str">
+        <v/>
+      </c>
+      <c t="str">
+        <v/>
+      </c>
+      <c t="str">
+        <v/>
+      </c>
+      <c t="str">
+        <v/>
+      </c>
+      <c t="str">
+        <v/>
+      </c>
+      <c t="str">
+        <v/>
+      </c>
+      <c t="str">
+        <v/>
+      </c>
+      <c t="str">
+        <v/>
+      </c>
+      <c t="str">
+        <v/>
+      </c>
+    </row>
+    <row>
+      <c t="str">
+        <v>4/8/2024</v>
+      </c>
+      <c t="str">
+        <v>Automation  Engineer E</v>
+      </c>
+      <c t="str">
+        <v>4/3/2024</v>
+      </c>
+      <c t="str">
+        <v>Service</v>
+      </c>
+      <c t="str">
+        <v/>
+      </c>
+      <c t="str">
+        <v/>
+      </c>
+      <c t="str">
+        <v>$0</v>
+      </c>
+      <c t="str">
+        <v>$0</v>
+      </c>
+      <c t="str">
+        <v>$0</v>
+      </c>
+    </row>
+    <row>
+      <c t="str">
+        <v>4/8/2024</v>
+      </c>
+      <c t="str">
+        <v>Automation  Engineer E</v>
+      </c>
+      <c t="str">
+        <v>4/3/2024</v>
+      </c>
+      <c t="str">
+        <v>Product</v>
+      </c>
+      <c t="str">
+        <v/>
+      </c>
+      <c t="str">
+        <v/>
+      </c>
+      <c t="str">
+        <v>$0</v>
+      </c>
+      <c t="str">
+        <v>$0</v>
+      </c>
+      <c t="str">
+        <v>$0</v>
+      </c>
+    </row>
+    <row>
+      <c t="str">
+        <v/>
+      </c>
+      <c t="str">
+        <v/>
+      </c>
+      <c t="str">
+        <v/>
+      </c>
+      <c t="str">
+        <v/>
+      </c>
+      <c t="str">
+        <v/>
+      </c>
+      <c t="str">
+        <v/>
+      </c>
+      <c t="str">
+        <v/>
+      </c>
+      <c t="str">
+        <v/>
+      </c>
+      <c t="str">
+        <v/>
+      </c>
+    </row>
+    <row>
+      <c t="str">
+        <v>4/8/2024</v>
+      </c>
+      <c t="str">
         <v>Test First Name Field Test Last Name Field</v>
       </c>
       <c t="str">
@@ -28371,6 +28943,93 @@
         <v>Test First Name Field Test Last Name Field</v>
       </c>
       <c t="str">
+        <v>4/13/2024</v>
+      </c>
+      <c t="str">
+        <v>Service</v>
+      </c>
+      <c t="str">
+        <v/>
+      </c>
+      <c t="str">
+        <v/>
+      </c>
+      <c t="str">
+        <v>$0</v>
+      </c>
+      <c t="str">
+        <v>$0</v>
+      </c>
+      <c t="str">
+        <v>$0</v>
+      </c>
+    </row>
+    <row>
+      <c t="str">
+        <v>4/8/2024</v>
+      </c>
+      <c t="str">
+        <v>Test First Name Field Test Last Name Field</v>
+      </c>
+      <c t="str">
+        <v>4/13/2024</v>
+      </c>
+      <c t="str">
+        <v>Product</v>
+      </c>
+      <c t="str">
+        <v/>
+      </c>
+      <c t="str">
+        <v/>
+      </c>
+      <c t="str">
+        <v>$0</v>
+      </c>
+      <c t="str">
+        <v>$0</v>
+      </c>
+      <c t="str">
+        <v>$0</v>
+      </c>
+    </row>
+    <row>
+      <c t="str">
+        <v/>
+      </c>
+      <c t="str">
+        <v/>
+      </c>
+      <c t="str">
+        <v/>
+      </c>
+      <c t="str">
+        <v/>
+      </c>
+      <c t="str">
+        <v/>
+      </c>
+      <c t="str">
+        <v/>
+      </c>
+      <c t="str">
+        <v/>
+      </c>
+      <c t="str">
+        <v/>
+      </c>
+      <c t="str">
+        <v/>
+      </c>
+    </row>
+    <row>
+      <c t="str">
+        <v>4/8/2024</v>
+      </c>
+      <c t="str">
+        <v>Test First Name Field Test Last Name Field</v>
+      </c>
+      <c t="str">
         <v>4/10/2024</v>
       </c>
       <c t="str">
@@ -31533,6 +32192,180 @@
       </c>
       <c t="str">
         <v>3/10/2024</v>
+      </c>
+      <c t="str">
+        <v>Product</v>
+      </c>
+      <c t="str">
+        <v/>
+      </c>
+      <c t="str">
+        <v/>
+      </c>
+      <c t="str">
+        <v>$0</v>
+      </c>
+      <c t="str">
+        <v>$0</v>
+      </c>
+      <c t="str">
+        <v>$0</v>
+      </c>
+    </row>
+    <row>
+      <c t="str">
+        <v/>
+      </c>
+      <c t="str">
+        <v/>
+      </c>
+      <c t="str">
+        <v/>
+      </c>
+      <c t="str">
+        <v/>
+      </c>
+      <c t="str">
+        <v/>
+      </c>
+      <c t="str">
+        <v/>
+      </c>
+      <c t="str">
+        <v/>
+      </c>
+      <c t="str">
+        <v/>
+      </c>
+      <c t="str">
+        <v/>
+      </c>
+    </row>
+    <row>
+      <c t="str">
+        <v>4/8/2024</v>
+      </c>
+      <c t="str">
+        <v>Automation  Engineer E</v>
+      </c>
+      <c t="str">
+        <v>4/3/2024</v>
+      </c>
+      <c t="str">
+        <v>Service</v>
+      </c>
+      <c t="str">
+        <v/>
+      </c>
+      <c t="str">
+        <v/>
+      </c>
+      <c t="str">
+        <v>$0</v>
+      </c>
+      <c t="str">
+        <v>$0</v>
+      </c>
+      <c t="str">
+        <v>$0</v>
+      </c>
+    </row>
+    <row>
+      <c t="str">
+        <v>4/8/2024</v>
+      </c>
+      <c t="str">
+        <v>Automation  Engineer E</v>
+      </c>
+      <c t="str">
+        <v>4/3/2024</v>
+      </c>
+      <c t="str">
+        <v>Product</v>
+      </c>
+      <c t="str">
+        <v/>
+      </c>
+      <c t="str">
+        <v/>
+      </c>
+      <c t="str">
+        <v>$0</v>
+      </c>
+      <c t="str">
+        <v>$0</v>
+      </c>
+      <c t="str">
+        <v>$0</v>
+      </c>
+    </row>
+    <row>
+      <c t="str">
+        <v/>
+      </c>
+      <c t="str">
+        <v/>
+      </c>
+      <c t="str">
+        <v/>
+      </c>
+      <c t="str">
+        <v/>
+      </c>
+      <c t="str">
+        <v/>
+      </c>
+      <c t="str">
+        <v/>
+      </c>
+      <c t="str">
+        <v/>
+      </c>
+      <c t="str">
+        <v/>
+      </c>
+      <c t="str">
+        <v/>
+      </c>
+    </row>
+    <row>
+      <c t="str">
+        <v>4/8/2024</v>
+      </c>
+      <c t="str">
+        <v>Automation  Engineer E</v>
+      </c>
+      <c t="str">
+        <v>4/3/2024</v>
+      </c>
+      <c t="str">
+        <v>Service</v>
+      </c>
+      <c t="str">
+        <v/>
+      </c>
+      <c t="str">
+        <v/>
+      </c>
+      <c t="str">
+        <v>$0</v>
+      </c>
+      <c t="str">
+        <v>$0</v>
+      </c>
+      <c t="str">
+        <v>$0</v>
+      </c>
+    </row>
+    <row>
+      <c t="str">
+        <v>4/8/2024</v>
+      </c>
+      <c t="str">
+        <v>Automation  Engineer E</v>
+      </c>
+      <c t="str">
+        <v>4/3/2024</v>
       </c>
       <c t="str">
         <v>Product</v>

</xml_diff>